<commit_message>
final version (as accepted by UWSpace)
</commit_message>
<xml_diff>
--- a/thesis/analysis/graphs/Xc comparison.xlsx
+++ b/thesis/analysis/graphs/Xc comparison.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/junjie/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ForrestLab\Dropbox\MSc-thesis\thesis\analysis\graphs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8F489240-BF8F-C644-B6BB-54C5669B55DB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76F3A1F1-F2B8-4116-A890-F8D769C1E3A5}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="840" windowWidth="27640" windowHeight="16540" xr2:uid="{B41E73A3-93BD-8C44-B5E6-2A6A1044C12A}"/>
+    <workbookView xWindow="420" yWindow="840" windowWidth="27645" windowHeight="16545" xr2:uid="{B41E73A3-93BD-8C44-B5E6-2A6A1044C12A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1067,7 +1067,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:numFmt formatCode="#\ ??/100" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2088,9 +2088,9 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2107,7 +2107,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>8.5069999999999997</v>
       </c>
@@ -2115,7 +2115,7 @@
         <v>0.33203045685279187</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>8.6771999999999991</v>
       </c>
@@ -2123,7 +2123,7 @@
         <v>0.3246700507614213</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>8.6820000000000004</v>
       </c>
@@ -2132,13 +2132,13 @@
         <v>0.54</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>8.8442000000000007</v>
       </c>
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>9</v>
       </c>
@@ -2147,7 +2147,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>9.0079999999999991</v>
       </c>
@@ -2155,7 +2155,7 @@
         <v>0.75939086294416236</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>9.1685999999999996</v>
       </c>
@@ -2163,7 +2163,7 @@
         <v>0.56903553299492382</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9.3260000000000005</v>
       </c>
@@ -2171,7 +2171,7 @@
         <v>0.42802030456852791</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9.4802</v>
       </c>
@@ -2179,7 +2179,7 @@
         <v>0.3184771573604061</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9.6311999999999998</v>
       </c>
@@ -2187,7 +2187,7 @@
         <v>0.53908629441624367</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9.7789999999999999</v>
       </c>
@@ -2195,13 +2195,13 @@
         <v>0.47766497461928931</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9.9236000000000004</v>
       </c>
       <c r="B13" s="1"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>10</v>
       </c>
@@ -2210,7 +2210,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>10.065</v>
       </c>
@@ -2218,7 +2218,7 @@
         <v>0.38020304568527924</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>10.338200000000001</v>
       </c>
@@ -2226,7 +2226,7 @@
         <v>0.49335025380710656</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>10.469999999999999</v>
       </c>
@@ -2234,7 +2234,7 @@
         <v>0.45294416243654823</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>10.598599999999999</v>
       </c>
@@ -2242,7 +2242,7 @@
         <v>0.5578680203045685</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>10.8462</v>
       </c>
@@ -2250,7 +2250,7 @@
         <v>0.56091370558375631</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>10.965199999999999</v>
       </c>
@@ -2258,7 +2258,7 @@
         <v>0.6675126903553299</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>11.081</v>
       </c>
@@ -2266,7 +2266,7 @@
         <v>0.61979695431472082</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>11.303000000000001</v>
       </c>
@@ -2274,13 +2274,13 @@
         <v>0.54467005076142128</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>11.5122</v>
       </c>
       <c r="B23" s="1"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>11.612</v>
       </c>
@@ -2288,7 +2288,7 @@
         <v>0.51472081218274113</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>11.802</v>
       </c>
@@ -2296,7 +2296,7 @@
         <v>0.47360406091370555</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>11.892199999999999</v>
       </c>
@@ -2304,7 +2304,7 @@
         <v>0.65888324873096449</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>11.979199999999999</v>
       </c>
@@ -2312,7 +2312,7 @@
         <v>0.47477157360406091</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>12.062999999999999</v>
       </c>
@@ -2320,7 +2320,7 @@
         <v>0.43771573604060915</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>12.143599999999999</v>
       </c>
@@ -2328,7 +2328,7 @@
         <v>0.51218274111675133</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>12.221</v>
       </c>
@@ -2336,7 +2336,7 @@
         <v>0.57411167512690353</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>12.366199999999999</v>
       </c>
@@ -2344,7 +2344,7 @@
         <v>0.60203045685279188</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>12.4986</v>
       </c>
@@ -2352,7 +2352,7 @@
         <v>0.60507614213197969</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>12.56</v>
       </c>
@@ -2360,7 +2360,7 @@
         <v>0.51522842639593913</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>12.6732</v>
       </c>
@@ -2368,7 +2368,7 @@
         <v>0.59086294416243657</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>12.725</v>
       </c>
@@ -2376,13 +2376,13 @@
         <v>0.62639593908629443</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>12.7736</v>
       </c>
       <c r="B36" s="1"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>12.818999999999999</v>
       </c>
@@ -2390,7 +2390,7 @@
         <v>0.55989847715736041</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>12.9002</v>
       </c>
@@ -2398,7 +2398,7 @@
         <v>0.60253807106598989</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>12.936</v>
       </c>
@@ -2406,7 +2406,7 @@
         <v>0.67563451776649741</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>13.227</v>
       </c>
@@ -2415,7 +2415,7 @@
         <v>0.68</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>15</v>
       </c>

</xml_diff>